<commit_message>
file düzenlendi. import from excel düzenlendi
</commit_message>
<xml_diff>
--- a/src/api/helper/file.xlsx
+++ b/src/api/helper/file.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Desktop\dev\src\api\helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERP\Desktop\dev\src\api\helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20400" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="TAPDK VAR DSD DE YOK" sheetId="1" r:id="rId1"/>
+    <sheet name="KAYIT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TAPDK VAR DSD DE YOK'!$A$1:$H$241</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KAYIT!$A$1:$H$242</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Bölgeler</t>
   </si>
@@ -73,6 +73,45 @@
   <si>
     <t>İSTANBUL=KARTAL,KADIKÖY,MALTEPE,PENDİK,TUZLA;
 KOCAELİ=DARICA</t>
+  </si>
+  <si>
+    <t>KOPUZ DIŞ</t>
+  </si>
+  <si>
+    <t>Nuray ÇELİK&lt;nuraycelik@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>Taner MARANGOZ&lt;tanermarangoz@kopuz.com.tr&gt;,
+Cemal KOPUZ&lt;cemal@kopuz.com.tr&gt;,
+Ahmet USTAOĞLU&lt;ahmet.ustaoglu@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>Özgür YILDIRIM&lt;ozguryildirim@kopuz.com.tr&gt;,
+Yavuz ELMAS&lt;yavuzelmas@kopuz.com.tr&gt;,
+Yalçın SÜZMETAŞ&lt;yalcinsuzmetas@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>KOPUZ İÇ</t>
+  </si>
+  <si>
+    <t>Seval TUNCER&lt;seval.tuncer@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>Tuncay KARAKAYA&lt;tuncaykarakaya@kopuz.com.tr&gt;,
+Vedat YURTSEVEN&lt;vedatyurduseven@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>Emre ÇİFTÇİOĞLU&lt;emreciftcioglu@kopuz.com.tr&gt;,
+İsmail KILIÇASLAN&lt;ismailkilicaslan@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>ASYA PAZARLAMA</t>
+  </si>
+  <si>
+    <t>Ramazan SARIYILDIZ&lt;asyapazarlama@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Melih BIYIKLI&lt;melihbiyikli@gmail.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -495,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,9 +547,9 @@
     <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52" style="1" customWidth="1"/>
-    <col min="7" max="7" width="53.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="54" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -544,7 +583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -573,71 +612,117 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+    <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>100</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5">
+        <v>605</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>100</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5">
+        <v>606</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>100</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5">
+        <v>607</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -672,6 +757,17 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
user aggretion tamam. read dist from excel tamam
</commit_message>
<xml_diff>
--- a/src/api/helper/file.xlsx
+++ b/src/api/helper/file.xlsx
@@ -15,17 +15,14 @@
     <sheet name="KAYIT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KAYIT!$A$1:$H$242</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KAYIT!$A$1:$H$246</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
-  <si>
-    <t>Bölgeler</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Bölge</t>
   </si>
@@ -46,9 +43,6 @@
   </si>
   <si>
     <t>OPERATÖR</t>
-  </si>
-  <si>
-    <t>KUZEY</t>
   </si>
   <si>
     <t>ASYA</t>
@@ -69,10 +63,6 @@
   </si>
   <si>
     <t>Bölge Şehir</t>
-  </si>
-  <si>
-    <t>İSTANBUL=KARTAL,KADIKÖY,MALTEPE,PENDİK,TUZLA;
-KOCAELİ=DARICA</t>
   </si>
   <si>
     <t>KOPUZ DIŞ</t>
@@ -112,6 +102,182 @@
   </si>
   <si>
     <t>Melih BIYIKLI&lt;melihbiyikli@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>GAZİANTEP</t>
+  </si>
+  <si>
+    <t>DÜNYA - GAZİANTEP</t>
+  </si>
+  <si>
+    <t>Taner SABAHLAR&lt;tsabahlar@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Bünyamin SEVER&lt;bunyamin027jti@gmail.com&gt;,
+Yasin İNAN&lt;yasininan27@hotmail.com&gt;</t>
+  </si>
+  <si>
+    <t>M.Kemal TANRIVERDİ&lt;jtigaziantep@dunyalimited.com&gt;</t>
+  </si>
+  <si>
+    <t>GAZİANTEP=ARABAN,KARKAMIŞ,NİZİP,OĞUZELİ,ŞAHİNBEY,ŞEHİTKAMİL,YAVUZELİ;</t>
+  </si>
+  <si>
+    <t>İSTANBUL=KARTAL,KADIKÖY,MALTEPE,PENDİK,TUZLA,ADALAR;
+KOCAELİ=DARICA,GEBZE</t>
+  </si>
+  <si>
+    <t>İSTANBUL=ATAŞEHİR,BEYKOZ,ÇATALCA,ÇEKMEKÖY,KADIKÖY,KARTAL,MALTEPE,PENDİK,SANCAKTEPE,ŞİLE,SULTANBEYLİ,TUZLA,ÜMRANİYE,ÜSKÜDAR;
+KOCAELİ=GEBZE</t>
+  </si>
+  <si>
+    <t>İSTANBUL=TUZLA;
+KOCAELİ=ÇAYIROVA,DARICA,DİLOVASI,GEBZE</t>
+  </si>
+  <si>
+    <t>İSTANBUL=ÜMRANİYE,ÜSKÜDAR,ATAŞEHİR,BEYKOZ,KADIKÖY;</t>
+  </si>
+  <si>
+    <t>DÜNYA - İSKENDERUN</t>
+  </si>
+  <si>
+    <t>Kemal SERİN&lt;kemalserin77@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Yusuf GÜLMEN&lt;jtiiskenderun@dunyalimited.com&gt;</t>
+  </si>
+  <si>
+    <t>HATAY=ARSUZ,BELEN,DÖRTYOL,İSKENDERUN;</t>
+  </si>
+  <si>
+    <t>DÜNYA - KAHRAMANMARAŞ</t>
+  </si>
+  <si>
+    <t>Muhammed NERGİZ&lt;dsmf.muhammednergiz@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Soner DEMİR&lt;jtikmaras@dunyalimited.com&gt;</t>
+  </si>
+  <si>
+    <t>Mustafa YAŞAR&lt;tte.mustafayasar@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>GAZİANTEP=İSLAHİYE,NURDAĞ;
+MALATYA=DARENDE,KULUNCAK;
+K.MARAŞ=AFŞİN,ANDIRIN,ÇAĞLAYANCERİT,DULKADİROĞLU,EKİNÖZÜ,ELBİSTAN,GÖKSUN,MERKEZ,NURHAK,ONİKİŞUBAT,PAZARCIK,TÜRKOĞLU;
+SİVAS=GÜRÜN</t>
+  </si>
+  <si>
+    <t>DÜNYA - ANTAKYA</t>
+  </si>
+  <si>
+    <t>Adnan AYTEKİN&lt;adnanxaytekin@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Murat ALTUĞ&lt;murataltugx@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Umut Cide&lt;jtiantakya@dunyalimited.com&gt;</t>
+  </si>
+  <si>
+    <t>HATAY=ALTINÖZÜ,ANTAKYA,BELEN,DEFNE,HASSA,KIRIKHAN,KUMLU,MERKEZ,REYHANLI,SAMANDAĞ,YAYLADAĞI,</t>
+  </si>
+  <si>
+    <t>ŞEKERCİ</t>
+  </si>
+  <si>
+    <t>Operatör&lt;sekerci.urfa@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Mehmet KÜÇÜK&lt;mehmetkucuk5563@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>ŞANLIURFA=AKÇAKALE,BİRECİK,BOZOVA,CEYLANPINAR,EYYÜBİYE,HALFETİ,HALİLİYE,HARRAN,HİLVAN,KARAKÖPRÜ,MERKEZ,SİVEREK,VİRANŞEHİR;</t>
+  </si>
+  <si>
+    <t>Murat YILDIRIM&lt;murat.yildirim@ongunemgin.com&gt;,
+Fatih YAŞA&lt;fatih.yasa@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Zeynep&lt;ofis.kocaeli@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Mehmet DURMAZ&lt;mehmet.durmaz@ongunemgin.com&gt;,
+Uğur SARAÇ&lt;ugur.sarac@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>KOCAELİ=BAŞİSKELE,DERİNCE,GÖLCÜK,KANDIRA,KARAMÜRSEL,KARTEPE,KÖRFEZ,MERKEZ,İZMİT</t>
+  </si>
+  <si>
+    <t>Mehmet ÖZEN&lt;mehmet.ozen@ongunemgin.com&gt;,
+Hamza ÇINAR&lt;hamza.cinar@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Alpay AYDIN&lt;alpay.aydin@ongunemgin.com&gt;,
+Fehmi DERTLİ&lt;fehmi.dertli@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Handan ERKAN&lt;ofis.sakarya@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>SAKARYA=ADAPAZARI,AKYAZI,ARİFİYE,ERENLER,FERİZLİ,GEYVE,HENDEK,KARAPÜRÇEK,KARASU,KAYNARCA,KOCAALİ,PAMUKOVA,SAPANCA,SERDİVAN,SÖĞÜTLÜ,TARAKLI</t>
+  </si>
+  <si>
+    <t>Alt Bölge</t>
+  </si>
+  <si>
+    <t>ONGUN - KOCAELİ</t>
+  </si>
+  <si>
+    <t>İZMİT</t>
+  </si>
+  <si>
+    <t>ONGUN - SAKARYA</t>
+  </si>
+  <si>
+    <t>ASYA BM</t>
+  </si>
+  <si>
+    <t>DOĞU BM</t>
+  </si>
+  <si>
+    <t>KOPUZ - BOLU</t>
+  </si>
+  <si>
+    <t>Zekeriye ÇALIŞKAN&lt;zekeriyacaliskanjti@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Sertaç ÖZSOY&lt;bolu.jti@kopuz.com.tr&gt;</t>
+  </si>
+  <si>
+    <t>Şafak ARABACI&lt;safakarabaci14@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>BOLU=DÖRTDİVAN,GEREDE,GÖYNÜK,KIBRISCIK,MENGEN,MUDURNU,SEBEN,YENİÇAĞA</t>
+  </si>
+  <si>
+    <t>GÜNEY BM</t>
+  </si>
+  <si>
+    <t>ADANA</t>
+  </si>
+  <si>
+    <t>ONGUN EMGİN - MERSİN</t>
+  </si>
+  <si>
+    <t>Operatör&lt;mersin@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Fatoş YÜRÜDEN&lt;fatosyuruden@ongunemgin.com&gt;,
+Yunus DÖNMEZ&lt;yunus.donmez@ongunemgin.com&gt;,
+Yılmaz OĞUZÖZKAN&lt;yilmaz.oguzozkan@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>Mete TAŞDEMİR&lt;mete.tasdemir@ongunemgin.com&gt;,
+Mehmet BİLGİÇ&lt;mehmet.bilgic@ongunemgin.com&gt;</t>
+  </si>
+  <si>
+    <t>MERSİN=AKDENİZ,ANAMUR,AYDINCIK,BOZYAZI,ÇAMLIYAYLA,ERDEMLİ,GÜLNAR,MERKEZ,MEZİTLİ,SİLİFKE,TARSUS,TOROSLAR,YENİŞEHİR</t>
   </si>
 </sst>
 </file>
@@ -159,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,21 +355,6 @@
       <right style="dashed">
         <color indexed="64"/>
       </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="dashed">
         <color indexed="64"/>
@@ -214,20 +365,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,22 +684,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="47.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="48.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="54" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -559,214 +707,422 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3401</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>100</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3402</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3403</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="I4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
         <v>100</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5">
-        <v>604</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5">
-        <v>100</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3404</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="4">
+        <v>200</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4101</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4">
+        <v>200</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4102</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="4">
+        <v>200</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4103</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="4">
+        <v>300</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="4">
+        <v>101</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5">
-        <v>605</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="C10" s="4">
+        <v>400</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2701</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5">
-        <v>100</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="5">
-        <v>606</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5">
-        <v>100</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5">
-        <v>607</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
+        <v>400</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2702</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4">
+        <v>400</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2703</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4">
+        <v>400</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2704</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4">
+        <v>400</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2705</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bayiler bulk tamamlandi. file düzenlendi
</commit_message>
<xml_diff>
--- a/src/api/helper/file.xlsx
+++ b/src/api/helper/file.xlsx
@@ -59,9 +59,6 @@
 Murat DEMİR&lt;demirmurat78@gmail.com&gt;</t>
   </si>
   <si>
-    <t>Zafer GENÇ&lt;zafergenc02@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Bölge Şehir</t>
   </si>
   <si>
@@ -120,13 +117,6 @@
     <t>M.Kemal TANRIVERDİ&lt;jtigaziantep@dunyalimited.com&gt;</t>
   </si>
   <si>
-    <t>GAZİANTEP=ARABAN,KARKAMIŞ,NİZİP,OĞUZELİ,ŞAHİNBEY,ŞEHİTKAMİL,YAVUZELİ;</t>
-  </si>
-  <si>
-    <t>İSTANBUL=KARTAL,KADIKÖY,MALTEPE,PENDİK,TUZLA,ADALAR;
-KOCAELİ=DARICA,GEBZE</t>
-  </si>
-  <si>
     <t>İSTANBUL=ATAŞEHİR,BEYKOZ,ÇATALCA,ÇEKMEKÖY,KADIKÖY,KARTAL,MALTEPE,PENDİK,SANCAKTEPE,ŞİLE,SULTANBEYLİ,TUZLA,ÜMRANİYE,ÜSKÜDAR;
 KOCAELİ=GEBZE</t>
   </si>
@@ -135,9 +125,6 @@
 KOCAELİ=ÇAYIROVA,DARICA,DİLOVASI,GEBZE</t>
   </si>
   <si>
-    <t>İSTANBUL=ÜMRANİYE,ÜSKÜDAR,ATAŞEHİR,BEYKOZ,KADIKÖY;</t>
-  </si>
-  <si>
     <t>DÜNYA - İSKENDERUN</t>
   </si>
   <si>
@@ -145,9 +132,6 @@
   </si>
   <si>
     <t>Yusuf GÜLMEN&lt;jtiiskenderun@dunyalimited.com&gt;</t>
-  </si>
-  <si>
-    <t>HATAY=ARSUZ,BELEN,DÖRTYOL,İSKENDERUN;</t>
   </si>
   <si>
     <t>DÜNYA - KAHRAMANMARAŞ</t>
@@ -180,9 +164,6 @@
     <t>Umut Cide&lt;jtiantakya@dunyalimited.com&gt;</t>
   </si>
   <si>
-    <t>HATAY=ALTINÖZÜ,ANTAKYA,BELEN,DEFNE,HASSA,KIRIKHAN,KUMLU,MERKEZ,REYHANLI,SAMANDAĞ,YAYLADAĞI,</t>
-  </si>
-  <si>
     <t>ŞEKERCİ</t>
   </si>
   <si>
@@ -190,9 +171,6 @@
   </si>
   <si>
     <t>Mehmet KÜÇÜK&lt;mehmetkucuk5563@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>ŞANLIURFA=AKÇAKALE,BİRECİK,BOZOVA,CEYLANPINAR,EYYÜBİYE,HALFETİ,HALİLİYE,HARRAN,HİLVAN,KARAKÖPRÜ,MERKEZ,SİVEREK,VİRANŞEHİR;</t>
   </si>
   <si>
     <t>Murat YILDIRIM&lt;murat.yildirim@ongunemgin.com&gt;,
@@ -278,6 +256,28 @@
   </si>
   <si>
     <t>MERSİN=AKDENİZ,ANAMUR,AYDINCIK,BOZYAZI,ÇAMLIYAYLA,ERDEMLİ,GÜLNAR,MERKEZ,MEZİTLİ,SİLİFKE,TARSUS,TOROSLAR,YENİŞEHİR</t>
+  </si>
+  <si>
+    <t>İSTANBUL=ÜMRANİYE,ÜSKÜDAR,ATAŞEHİR,BEYKOZ,KADIKÖY</t>
+  </si>
+  <si>
+    <t>GAZİANTEP=ARABAN,KARKAMIŞ,NİZİP,OĞUZELİ,ŞAHİNBEY,ŞEHİTKAMİL,YAVUZELİ</t>
+  </si>
+  <si>
+    <t>HATAY=ARSUZ,BELEN,DÖRTYOL,İSKENDERUN</t>
+  </si>
+  <si>
+    <t>HATAY=ALTINÖZÜ,ANTAKYA,BELEN,DEFNE,HASSA,KIRIKHAN,KUMLU,MERKEZ,REYHANLI,SAMANDAĞ,YAYLADAĞI</t>
+  </si>
+  <si>
+    <t>ŞANLIURFA=AKÇAKALE,BİRECİK,BOZOVA,CEYLANPINAR,EYYÜBİYE,HALFETİ,HALİLİYE,HARRAN,HİLVAN,KARAKÖPRÜ,MERKEZ,SİVEREK,VİRANŞEHİR</t>
+  </si>
+  <si>
+    <t>İSTANBUL=KARTAL,KADIKÖY,MALTEPE,PENDİK,TUZLA,ADALAR;
+KOCAELİ=DARICA,GEBZE;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zafer GENÇ &lt; zafergenc02@gmail.com&gt; </t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -707,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -728,12 +730,12 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -754,15 +756,15 @@
         <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -771,25 +773,25 @@
         <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4">
         <v>3402</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -798,27 +800,27 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4">
         <v>3403</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -827,279 +829,279 @@
         <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4">
         <v>3404</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4">
         <v>200</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E6" s="4">
         <v>4101</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4">
         <v>200</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4">
         <v>4102</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4">
         <v>200</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E8" s="4">
         <v>4103</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4">
         <v>300</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4">
         <v>101</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4">
         <v>400</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4">
         <v>2701</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4">
         <v>400</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" s="4">
         <v>2702</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4">
         <v>400</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" s="4">
         <v>2703</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4">
         <v>400</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E13" s="4">
         <v>2704</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <v>400</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4">
         <v>2705</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>